<commit_message>
Modifiche generali per il funzionamento download
</commit_message>
<xml_diff>
--- a/templates/GestioneSalariOspedale.xlsx
+++ b/templates/GestioneSalariOspedale.xlsx
@@ -161,9 +161,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -242,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -253,6 +254,10 @@
     <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -592,7 +597,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="F4" activeCellId="1" sqref="A4 F4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -636,22 +641,22 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="5" t="e">
+      <c r="F4" s="10" t="e">
         <f>D4 +( E4 * 10)</f>
         <v>#VALUE!</v>
       </c>
@@ -662,12 +667,12 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="7">
+      <c r="D5" s="12">
         <f>SUM(D4)</f>
         <v>0</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="7" t="e">
+      <c r="F5" s="12" t="e">
         <f>SUM(F4)</f>
         <v>#VALUE!</v>
       </c>

</xml_diff>